<commit_message>
first two MR-style passes
</commit_message>
<xml_diff>
--- a/data/generator.xlsx
+++ b/data/generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="960" windowWidth="20740" windowHeight="17420" tabRatio="500"/>
+    <workbookView xWindow="7960" yWindow="680" windowWidth="20740" windowHeight="17420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ts1" sheetId="1" r:id="rId1"/>
@@ -47,8 +47,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd\ hh:mm:ss\.ss"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\Thh:mm:ss\.ss\Z"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -148,10 +148,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -528,13 +528,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -562,114 +562,114 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3">
-        <f ca="1">RANDBETWEEN(300,1800)/86400+A2</f>
-        <v>41640.504641203705</v>
+        <f t="shared" ref="A3:A10" ca="1" si="0">RANDBETWEEN(300,1800)/86400+A2</f>
+        <v>41640.512604166666</v>
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(-30,30)/3600+B2</f>
-        <v>37.991666666666667</v>
+        <v>37.996944444444445</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(-30,30)/3600+C2</f>
-        <v>-135.00805555555556</v>
+        <v>-135.00638888888889</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3">
-        <f ca="1">RANDBETWEEN(300,1800)/86400+A3</f>
-        <v>41640.522361111114</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41640.531631944446</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B10" ca="1" si="0">RANDBETWEEN(-30,30)/3600+B3</f>
-        <v>37.991388888888892</v>
+        <f t="shared" ref="B4:B10" ca="1" si="1">RANDBETWEEN(-30,30)/3600+B3</f>
+        <v>38.003611111111113</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C10" ca="1" si="1">RANDBETWEEN(-30,30)/3600+C3</f>
-        <v>-135.01083333333332</v>
+        <f t="shared" ref="C4:C10" ca="1" si="2">RANDBETWEEN(-30,30)/3600+C3</f>
+        <v>-135.01166666666668</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3">
-        <f ca="1">RANDBETWEEN(300,1800)/86400+A4</f>
-        <v>41640.534930555557</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41640.552152777782</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>37.989444444444445</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>38.000277777777782</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>-135.01249999999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-135.01055555555558</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3">
-        <f ca="1">RANDBETWEEN(300,1800)/86400+A5</f>
-        <v>41640.540219907409</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41640.571446759262</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>37.985833333333332</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>37.994444444444447</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>-135.01694444444442</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-135.00805555555559</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3">
-        <f ca="1">RANDBETWEEN(300,1800)/86400+A6</f>
-        <v>41640.552615740744</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41640.586122685185</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>37.982222222222219</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>37.998888888888892</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>-135.01111111111109</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-135.01277777777781</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3">
-        <f ca="1">RANDBETWEEN(300,1800)/86400+A7</f>
-        <v>41640.55809027778</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41640.59302083333</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>37.974999999999994</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>37.991111111111117</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>-135.00833333333333</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-135.01611111111114</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3">
-        <f ca="1">RANDBETWEEN(300,1800)/86400+A8</f>
-        <v>41640.564664351856</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41640.597141203703</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>37.977777777777774</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>37.982777777777784</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>-135.0011111111111</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-135.01000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3">
-        <f ca="1">RANDBETWEEN(300,1800)/86400+A9</f>
-        <v>41640.579409722224</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41640.611990740741</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>37.983888888888885</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>37.988055555555562</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>-134.99944444444444</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-135.00527777777779</v>
       </c>
     </row>
   </sheetData>
@@ -687,13 +687,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -716,7 +716,7 @@
     <row r="3" spans="1:2">
       <c r="A3" s="3">
         <f ca="1">RANDBETWEEN(300,1800)/86400+A2</f>
-        <v>41640.511886574081</v>
+        <v>41640.504907407412</v>
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(-6,6)/10+B2</f>
@@ -726,17 +726,17 @@
     <row r="4" spans="1:2">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A10" ca="1" si="0">RANDBETWEEN(300,1800)/86400+A3</f>
-        <v>41640.5312962963</v>
+        <v>41640.5163425926</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B10" ca="1" si="1">RANDBETWEEN(-6,6)/10+B3</f>
-        <v>14.1</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>41640.535682870373</v>
+        <v>41640.536643518528</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
@@ -746,51 +746,51 @@
     <row r="6" spans="1:2">
       <c r="A6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>41640.556111111116</v>
+        <v>41640.543032407419</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>13.6</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>41640.565347222226</v>
+        <v>41640.558067129641</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>13.5</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>41640.575185185189</v>
+        <v>41640.564074074086</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>12.9</v>
+        <v>14.799999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>41640.594189814816</v>
+        <v>41640.579085648162</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>13.3</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>41640.612812500003</v>
+        <v>41640.597673611126</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>12.700000000000001</v>
+        <v>13.799999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -809,12 +809,12 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -837,82 +837,82 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3">
-        <f>A2+15/60/24</f>
+        <f t="shared" ref="A3:A10" si="0">A2+15/60/24</f>
         <v>41640.489583333328</v>
       </c>
       <c r="B3" s="1">
         <f ca="1">RANDBETWEEN(-4,4)/10+B2</f>
-        <v>10.1</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3">
-        <f>A3+15/60/24</f>
+        <f t="shared" si="0"/>
         <v>41640.499999999993</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B10" ca="1" si="0">RANDBETWEEN(-4,4)/10+B3</f>
+        <f t="shared" ref="B4:B10" ca="1" si="1">RANDBETWEEN(-4,4)/10+B3</f>
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3">
-        <f>A4+15/60/24</f>
+        <f t="shared" si="0"/>
         <v>41640.510416666657</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10.199999999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3">
-        <f>A5+15/60/24</f>
+        <f t="shared" si="0"/>
         <v>41640.520833333321</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10.6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>9.2999999999999989</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3">
-        <f>A6+15/60/24</f>
+        <f t="shared" si="0"/>
         <v>41640.531249999985</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>9.6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3">
-        <f>A7+15/60/24</f>
+        <f t="shared" si="0"/>
         <v>41640.54166666665</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11.2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>9.6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3">
-        <f>A8+15/60/24</f>
+        <f t="shared" si="0"/>
         <v>41640.552083333314</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10.799999999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>9.6</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3">
-        <f>A9+15/60/24</f>
+        <f t="shared" si="0"/>
         <v>41640.562499999978</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10.899999999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>9.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>